<commit_message>
Added figures with fMRIprep registration
</commit_message>
<xml_diff>
--- a/Figures/Error calc.xlsx
+++ b/Figures/Error calc.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\Residency\Research\FIDs Study\Github\afids_parkinsons\Figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Documents\GitHub\afids_parkinsons\Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00175F34-2859-41B8-9403-F3B84EA478E8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DF7465-3D8C-4D73-AEAC-9D89E89F72F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2610" windowWidth="21600" windowHeight="11423" activeTab="1" xr2:uid="{18484CF3-349D-466C-A8F4-E3C083C98DEB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{18484CF3-349D-466C-A8F4-E3C083C98DEB}"/>
   </bookViews>
   <sheets>
     <sheet name="AFLE" sheetId="1" r:id="rId1"/>
     <sheet name="AFRE" sheetId="2" r:id="rId2"/>
+    <sheet name="AFRE (fMRIprep)" sheetId="3" r:id="rId3"/>
+    <sheet name="Summary" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
   <si>
     <t>FID</t>
   </si>
@@ -57,13 +61,33 @@
   <si>
     <t>RC</t>
   </si>
+  <si>
+    <t>Fiducial</t>
+  </si>
+  <si>
+    <t>Patient Space</t>
+  </si>
+  <si>
+    <t>MNI Space</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -79,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,12 +111,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,6 +831,407 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-45C6-44C7-866E-F989A29766C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="50"/>
+        <c:overlap val="-27"/>
+        <c:axId val="427638896"/>
+        <c:axId val="356058224"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="427638896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="356058224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="356058224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427638896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="plus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>AFRE!$I$2:$I$33</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="32"/>
+                  <c:pt idx="0">
+                    <c:v>1.3196332775866899</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.2046081225858001</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.7318526841003501</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.08459364499886</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.3929137723037801</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.54208258257075</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.50003628548617</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.0448921498707602</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.0846167606711301</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1.63733499835594</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>1.99594421551857</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1.9780582421336099</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.0146981836608302</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.49452932617149</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>3.4382245408655399</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>3.4564742224650402</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>2.6317239597535602</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>2.2634427699884498</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.5355326184312399</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1.3319660392496</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>2.0612150301566001</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>2.12101192554633</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>2.4309683482161</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>2.6874199516931401</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>2.7252361362164699</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>3.3939916009129498</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>1.71402038929519</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>1.96276044218197</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>2.9541950338679501</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>3.1517998280833499</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
+                    <c:v>1.85446821583761</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>1.67648617828841</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>'AFRE (fMRIprep)'!$G$2:$G$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1.1014064201934737</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0377537949507838</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.105285451752068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8252816255830062</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0909550630433236</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0957687432673877</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2261931545799003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8699602551428023</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.0054840162432259</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.2644772319954942</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0300353389355323</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0147233106507998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1113185678691502</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.406890392989824</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.3473568054388183</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.1919625234490625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.2034767724297715</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.9523681912794242</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.5370645339501978</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.391284479921866</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.6053985320944575</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.2277420670840136</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.9290472219986903</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.1651092381726702</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.3965410438593207</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.7884760650634979</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.4905254528387899</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.2050549617434276</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.736525861999854</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.3296290481171296</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.6198390457545537</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.5814985495801759</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1154-4470-971B-3D68D6D02DBA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -992,6 +1439,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1496,6 +1983,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2060,6 +3050,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E061E8B5-F581-441B-9720-202A0B6DC275}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>569120</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>71439</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EE373E0-4D6B-4E8C-99D4-71C915AD2CA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2381,13 +3414,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22304D9-F8AF-4C40-BA43-F70F61C76FD7}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E58" sqref="A52:E58"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2413,7 +3446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2440,7 +3473,7 @@
         <v>0.60087772213935098</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2467,7 +3500,7 @@
         <v>0.29475468750790401</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2494,7 +3527,7 @@
         <v>0.58830697324466796</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2521,7 +3554,7 @@
         <v>0.44147759444463103</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2548,7 +3581,7 @@
         <v>0.70774337023607303</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2575,7 +3608,7 @@
         <v>0.77281571537741001</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2602,7 +3635,7 @@
         <v>0.87712004070392102</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2629,7 +3662,7 @@
         <v>0.89526119977700602</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2656,7 +3689,7 @@
         <v>0.97949788862765996</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2683,7 +3716,7 @@
         <v>0.92472504788955501</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2710,7 +3743,7 @@
         <v>0.40640654078738497</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2737,7 +3770,7 @@
         <v>0.413257486738488</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2764,7 +3797,7 @@
         <v>0.447976793714366</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2791,7 +3824,7 @@
         <v>0.75087232450117303</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2818,7 +3851,7 @@
         <v>1.6663752481357199</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2845,7 +3878,7 @@
         <v>1.6580239774665599</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2872,7 +3905,7 @@
         <v>1.3564883668760499</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2899,7 +3932,7 @@
         <v>0.92338362946604302</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2926,7 +3959,7 @@
         <v>0.75427645029030599</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2953,7 +3986,7 @@
         <v>0.69033432237493098</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2980,7 +4013,7 @@
         <v>1.0003277001697399</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3007,7 +4040,7 @@
         <v>1.42800891625922</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3034,7 +4067,7 @@
         <v>1.1897235733010001</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3061,7 +4094,7 @@
         <v>1.4655201750556901</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3088,7 +4121,7 @@
         <v>1.6714100194671899</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3115,7 +4148,7 @@
         <v>1.8475833442023699</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3142,7 +4175,7 @@
         <v>1.0572847661142299</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3169,7 +4202,7 @@
         <v>1.0241302236516401</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3196,7 +4229,7 @@
         <v>1.4676569959415999</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3223,7 +4256,7 @@
         <v>1.4115303017377101</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3250,7 +4283,7 @@
         <v>1.1370663159027301</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3277,7 +4310,7 @@
         <v>1.0958001125948</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -3320,13 +4353,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366FFB22-9D07-4899-BBED-03AC8511902B}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3352,7 +4385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3379,7 +4412,7 @@
         <v>1.3196332775866899</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3406,7 +4439,7 @@
         <v>1.2046081225858001</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3433,7 +4466,7 @@
         <v>1.7318526841003501</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3460,7 +4493,7 @@
         <v>2.08459364499886</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3487,7 +4520,7 @@
         <v>1.3929137723037801</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3514,7 +4547,7 @@
         <v>1.54208258257075</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3541,7 +4574,7 @@
         <v>1.50003628548617</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3568,7 +4601,7 @@
         <v>2.0448921498707602</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3595,7 +4628,7 @@
         <v>2.0846167606711301</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3622,7 +4655,7 @@
         <v>1.63733499835594</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3649,7 +4682,7 @@
         <v>1.99594421551857</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3676,7 +4709,7 @@
         <v>1.9780582421336099</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3703,7 +4736,7 @@
         <v>2.0146981836608302</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3730,7 +4763,7 @@
         <v>1.49452932617149</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3757,7 +4790,7 @@
         <v>3.4382245408655399</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3784,7 +4817,7 @@
         <v>3.4564742224650402</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3811,7 +4844,7 @@
         <v>2.6317239597535602</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3838,7 +4871,7 @@
         <v>2.2634427699884498</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3865,7 +4898,7 @@
         <v>1.5355326184312399</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3892,7 +4925,7 @@
         <v>1.3319660392496</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3919,7 +4952,7 @@
         <v>2.0612150301566001</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3946,7 +4979,7 @@
         <v>2.12101192554633</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3973,7 +5006,7 @@
         <v>2.4309683482161</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4000,7 +5033,7 @@
         <v>2.6874199516931401</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4027,7 +5060,7 @@
         <v>2.7252361362164699</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4054,7 +5087,7 @@
         <v>3.3939916009129498</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4081,7 +5114,7 @@
         <v>1.71402038929519</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4108,7 +5141,7 @@
         <v>1.96276044218197</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4135,7 +5168,7 @@
         <v>2.9541950338679501</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4162,7 +5195,7 @@
         <v>3.1517998280833499</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4189,7 +5222,7 @@
         <v>1.85446821583761</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4216,7 +5249,7 @@
         <v>1.67648617828841</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -4253,4 +5286,2184 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEF7006-1D20-4D3E-95F7-6E519B242F5B}">
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D36" zoomScale="113" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1.78486017540908</v>
+      </c>
+      <c r="C2">
+        <v>0.80480363827095003</v>
+      </c>
+      <c r="D2">
+        <v>0.83689502036837804</v>
+      </c>
+      <c r="E2">
+        <v>1.208022780014</v>
+      </c>
+      <c r="F2">
+        <v>0.87245048690496096</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE(B2:F2)</f>
+        <v>1.1014064201934737</v>
+      </c>
+      <c r="I2">
+        <v>1.0545756470888199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1.9610522800841199</v>
+      </c>
+      <c r="C3">
+        <v>2.1559429562824</v>
+      </c>
+      <c r="D3">
+        <v>2.0096177497046601</v>
+      </c>
+      <c r="E3">
+        <v>2.0097379846867498</v>
+      </c>
+      <c r="F3">
+        <v>2.0524180039959901</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G33" si="0">AVERAGE(B3:F3)</f>
+        <v>2.0377537949507838</v>
+      </c>
+      <c r="I3">
+        <v>1.2644726158938</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2.82006288751891</v>
+      </c>
+      <c r="C4">
+        <v>1.6100697767788501</v>
+      </c>
+      <c r="D4">
+        <v>2.09739028674817</v>
+      </c>
+      <c r="E4">
+        <v>2.6337594070980201</v>
+      </c>
+      <c r="F4">
+        <v>1.36514490061639</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>2.105285451752068</v>
+      </c>
+      <c r="I4">
+        <v>1.5493784975548399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3.0928817134730799</v>
+      </c>
+      <c r="C5">
+        <v>3.5696054093707801</v>
+      </c>
+      <c r="D5">
+        <v>2.8198163780585999</v>
+      </c>
+      <c r="E5">
+        <v>2.2590931033000099</v>
+      </c>
+      <c r="F5">
+        <v>2.38501152371256</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>2.8252816255830062</v>
+      </c>
+      <c r="I5">
+        <v>1.35035883880706</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1.9470607042468999</v>
+      </c>
+      <c r="C6">
+        <v>2.4736805811335998</v>
+      </c>
+      <c r="D6">
+        <v>1.6703402259037099</v>
+      </c>
+      <c r="E6">
+        <v>1.9322172068694401</v>
+      </c>
+      <c r="F6">
+        <v>2.4314765970629701</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>2.0909550630433236</v>
+      </c>
+      <c r="I6">
+        <v>1.14328648932295</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3.8542593421858702</v>
+      </c>
+      <c r="C7">
+        <v>2.89092042162968</v>
+      </c>
+      <c r="D7">
+        <v>2.9502180762336301</v>
+      </c>
+      <c r="E7">
+        <v>2.7109416446082499</v>
+      </c>
+      <c r="F7">
+        <v>3.0725042316795101</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>3.0957687432673877</v>
+      </c>
+      <c r="I7">
+        <v>1.5203069567115599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4.1452605998493404</v>
+      </c>
+      <c r="C8">
+        <v>2.7358141564691998</v>
+      </c>
+      <c r="D8">
+        <v>3.0979688933104299</v>
+      </c>
+      <c r="E8">
+        <v>3.0281033527319701</v>
+      </c>
+      <c r="F8">
+        <v>3.1238187705385601</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3.2261931545799003</v>
+      </c>
+      <c r="I8">
+        <v>1.74614022912149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3.5555312684255802</v>
+      </c>
+      <c r="C9">
+        <v>2.29922526099825</v>
+      </c>
+      <c r="D9">
+        <v>3.4004030957965399</v>
+      </c>
+      <c r="E9">
+        <v>2.7497145625986801</v>
+      </c>
+      <c r="F9">
+        <v>2.34492708789496</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>2.8699602551428023</v>
+      </c>
+      <c r="I9">
+        <v>1.66695149547249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3.8923288322851302</v>
+      </c>
+      <c r="C10">
+        <v>2.5712216238752101</v>
+      </c>
+      <c r="D10">
+        <v>3.7175992265697499</v>
+      </c>
+      <c r="E10">
+        <v>2.31608123932152</v>
+      </c>
+      <c r="F10">
+        <v>2.5301891591645198</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>3.0054840162432259</v>
+      </c>
+      <c r="I10">
+        <v>1.81595048530706</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>4.1239216644161001</v>
+      </c>
+      <c r="C11">
+        <v>4.2460893593343298</v>
+      </c>
+      <c r="D11">
+        <v>4.5094762478633497</v>
+      </c>
+      <c r="E11">
+        <v>3.3769044107591601</v>
+      </c>
+      <c r="F11">
+        <v>5.06599447760453</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>4.2644772319954942</v>
+      </c>
+      <c r="I11">
+        <v>1.99130225128418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1.8839188871175401</v>
+      </c>
+      <c r="C12">
+        <v>2.0959568776484399</v>
+      </c>
+      <c r="D12">
+        <v>2.1249824511533202</v>
+      </c>
+      <c r="E12">
+        <v>1.70775349761882</v>
+      </c>
+      <c r="F12">
+        <v>2.3375649811395398</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2.0300353389355323</v>
+      </c>
+      <c r="I12">
+        <v>1.0788543447296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1.79795405652894</v>
+      </c>
+      <c r="C13">
+        <v>2.35393989702454</v>
+      </c>
+      <c r="D13">
+        <v>2.0218708624509101</v>
+      </c>
+      <c r="E13">
+        <v>1.6029045161250299</v>
+      </c>
+      <c r="F13">
+        <v>2.2969472211245798</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>2.0147233106507998</v>
+      </c>
+      <c r="I13">
+        <v>1.0373284908842999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1.82050284843821</v>
+      </c>
+      <c r="C14">
+        <v>2.5070576078933602</v>
+      </c>
+      <c r="D14">
+        <v>2.1720234675527599</v>
+      </c>
+      <c r="E14">
+        <v>1.7092515832966499</v>
+      </c>
+      <c r="F14">
+        <v>2.34775733216477</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>2.1113185678691502</v>
+      </c>
+      <c r="I14">
+        <v>1.1138685141172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>3.8247402703765299</v>
+      </c>
+      <c r="C15">
+        <v>3.6721295886615302</v>
+      </c>
+      <c r="D15">
+        <v>3.4994863684481499</v>
+      </c>
+      <c r="E15">
+        <v>2.7013354249416901</v>
+      </c>
+      <c r="F15">
+        <v>3.33676031252122</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>3.406890392989824</v>
+      </c>
+      <c r="I15">
+        <v>1.7544452845530301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>6.7470458375818998</v>
+      </c>
+      <c r="C16">
+        <v>2.4983612040166299</v>
+      </c>
+      <c r="D16">
+        <v>2.4945401238555398</v>
+      </c>
+      <c r="E16">
+        <v>2.67747561756509</v>
+      </c>
+      <c r="F16">
+        <v>2.3193612441749298</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>3.3473568054388183</v>
+      </c>
+      <c r="I16">
+        <v>3.2938886633022699</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>6.6290864937861</v>
+      </c>
+      <c r="C17">
+        <v>2.17061392646078</v>
+      </c>
+      <c r="D17">
+        <v>2.2982210262791098</v>
+      </c>
+      <c r="E17">
+        <v>2.6148505538459701</v>
+      </c>
+      <c r="F17">
+        <v>2.2470406168733499</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>3.1919625234490625</v>
+      </c>
+      <c r="I17">
+        <v>3.48062829524374</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>3.9832476186124901</v>
+      </c>
+      <c r="C18">
+        <v>2.8650957736902498</v>
+      </c>
+      <c r="D18">
+        <v>2.9264073230000198</v>
+      </c>
+      <c r="E18">
+        <v>3.0106700630624799</v>
+      </c>
+      <c r="F18">
+        <v>3.23196308378362</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>3.2034767724297715</v>
+      </c>
+      <c r="I18">
+        <v>2.4649685796854701</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>3.3264832384933798</v>
+      </c>
+      <c r="C19">
+        <v>2.6809462305538601</v>
+      </c>
+      <c r="D19">
+        <v>2.8992201282721699</v>
+      </c>
+      <c r="E19">
+        <v>2.8689095465812899</v>
+      </c>
+      <c r="F19">
+        <v>2.9862818124964199</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>2.9523681912794242</v>
+      </c>
+      <c r="I19">
+        <v>2.0829686784909498</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2.75704110784954</v>
+      </c>
+      <c r="C20">
+        <v>2.6710445350954601</v>
+      </c>
+      <c r="D20">
+        <v>2.3918748562115</v>
+      </c>
+      <c r="E20">
+        <v>2.4696116099780201</v>
+      </c>
+      <c r="F20">
+        <v>2.3957505606164702</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>2.5370645339501978</v>
+      </c>
+      <c r="I20">
+        <v>1.36100957735988</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>3.6842646762848199</v>
+      </c>
+      <c r="C21">
+        <v>3.2891534279840702</v>
+      </c>
+      <c r="D21">
+        <v>2.6846258398845002</v>
+      </c>
+      <c r="E21">
+        <v>4.1572253680875599</v>
+      </c>
+      <c r="F21">
+        <v>3.1411530873683802</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>3.391284479921866</v>
+      </c>
+      <c r="I21">
+        <v>1.14268601929381</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>3.4376094969164601</v>
+      </c>
+      <c r="C22">
+        <v>2.3455670050798201</v>
+      </c>
+      <c r="D22">
+        <v>2.6268572504845702</v>
+      </c>
+      <c r="E22">
+        <v>2.31001487738077</v>
+      </c>
+      <c r="F22">
+        <v>2.3069440306106701</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>2.6053985320944575</v>
+      </c>
+      <c r="I22">
+        <v>1.7344561114160399</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>3.9347410623159398</v>
+      </c>
+      <c r="C23">
+        <v>2.8980178902865501</v>
+      </c>
+      <c r="D23">
+        <v>2.80656243323401</v>
+      </c>
+      <c r="E23">
+        <v>3.6155676157663099</v>
+      </c>
+      <c r="F23">
+        <v>2.8838213338172598</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>3.2277420670840136</v>
+      </c>
+      <c r="I23">
+        <v>2.3629380897714301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>5.0707915685701499</v>
+      </c>
+      <c r="C24">
+        <v>5.94654380430097</v>
+      </c>
+      <c r="D24">
+        <v>5.6232532537062898</v>
+      </c>
+      <c r="E24">
+        <v>4.2589561316789402</v>
+      </c>
+      <c r="F24">
+        <v>3.7456913517371002</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>4.9290472219986903</v>
+      </c>
+      <c r="I24">
+        <v>3.4698611960608901</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>5.2078639892482004</v>
+      </c>
+      <c r="C25">
+        <v>5.9083466572263301</v>
+      </c>
+      <c r="D25">
+        <v>5.7914442713119803</v>
+      </c>
+      <c r="E25">
+        <v>4.4858001105542398</v>
+      </c>
+      <c r="F25">
+        <v>4.4320911625225996</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>5.1651092381726702</v>
+      </c>
+      <c r="I25">
+        <v>2.23732809069051</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>5.12454057017335</v>
+      </c>
+      <c r="C26">
+        <v>4.8552483606402399</v>
+      </c>
+      <c r="D26">
+        <v>4.7431986916207798</v>
+      </c>
+      <c r="E26">
+        <v>3.7832962481091199</v>
+      </c>
+      <c r="F26">
+        <v>3.4764213487531102</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>4.3965410438593207</v>
+      </c>
+      <c r="I26">
+        <v>2.69548725642376</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>5.9137763747831</v>
+      </c>
+      <c r="C27">
+        <v>5.5505927500307699</v>
+      </c>
+      <c r="D27">
+        <v>5.3080915455741398</v>
+      </c>
+      <c r="E27">
+        <v>3.4665543845086302</v>
+      </c>
+      <c r="F27">
+        <v>3.70336527042085</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>4.7884760650634979</v>
+      </c>
+      <c r="I27">
+        <v>3.2672332340119601</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>3.47065843251091</v>
+      </c>
+      <c r="C28">
+        <v>3.1388346857961098</v>
+      </c>
+      <c r="D28">
+        <v>3.7947675496617501</v>
+      </c>
+      <c r="E28">
+        <v>4.0848047842796502</v>
+      </c>
+      <c r="F28">
+        <v>2.9635618119455298</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>3.4905254528387899</v>
+      </c>
+      <c r="I28">
+        <v>1.8869085069851099</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>4.1011521019278199</v>
+      </c>
+      <c r="C29">
+        <v>4.6452501715453298</v>
+      </c>
+      <c r="D29">
+        <v>4.3175487534825097</v>
+      </c>
+      <c r="E29">
+        <v>4.2876615097480597</v>
+      </c>
+      <c r="F29">
+        <v>3.67366227201342</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>4.2050549617434276</v>
+      </c>
+      <c r="I29">
+        <v>1.80908943619927</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>6.7964050299660901</v>
+      </c>
+      <c r="C30">
+        <v>6.0184144548066696</v>
+      </c>
+      <c r="D30">
+        <v>6.7119025356693696</v>
+      </c>
+      <c r="E30">
+        <v>6.7995700121117499</v>
+      </c>
+      <c r="F30">
+        <v>7.3563372774453901</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>6.736525861999854</v>
+      </c>
+      <c r="I30">
+        <v>2.9456997705349202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>7.17390718785225</v>
+      </c>
+      <c r="C31">
+        <v>6.7238484030253902</v>
+      </c>
+      <c r="D31">
+        <v>7.7698452579760398</v>
+      </c>
+      <c r="E31">
+        <v>7.2998401952804102</v>
+      </c>
+      <c r="F31">
+        <v>7.6807041964515603</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>7.3296290481171296</v>
+      </c>
+      <c r="I31">
+        <v>3.3691794399358002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>4.8619588276150401</v>
+      </c>
+      <c r="C32">
+        <v>1.80645111727275</v>
+      </c>
+      <c r="D32">
+        <v>2.1482469286030601</v>
+      </c>
+      <c r="E32">
+        <v>1.9492018651459</v>
+      </c>
+      <c r="F32">
+        <v>2.3333364901360198</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>2.6198390457545537</v>
+      </c>
+      <c r="I32">
+        <v>1.9249835648595199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>4.5802109830582598</v>
+      </c>
+      <c r="C33">
+        <v>1.9996289746312399</v>
+      </c>
+      <c r="D33">
+        <v>1.97710376966057</v>
+      </c>
+      <c r="E33">
+        <v>2.2057816725811801</v>
+      </c>
+      <c r="F33">
+        <v>2.1447673479696299</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>2.5814985495801759</v>
+      </c>
+      <c r="I33">
+        <v>1.8460526015158001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <f>AVERAGE(B2:B33)</f>
+        <v>3.9782850039969104</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:F34" si="1">AVERAGE(C2:C33)</f>
+        <v>3.2499505164941982</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>3.3200562465203212</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>3.0716129025073546</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>3.0807881057894173</v>
+      </c>
+      <c r="G34">
+        <f>AVERAGE(G2:G33)</f>
+        <v>3.3401385550616407</v>
+      </c>
+      <c r="I34">
+        <f>AVERAGE(I2:I33)</f>
+        <v>1.9832058516446722</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9C33D4-1919-4569-A4A3-BFD8417E78E0}">
+  <dimension ref="A1:K35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScale="70" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="7.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="5.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1.1228720500090701</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.45928282655605501</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.60220490868468102</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.73580081012669296</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.53693463516500095</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1.78486017540908</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.80480363827095003</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0.83689502036837804</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1.208022780014</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.87245048690496096</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.88672338209121604</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.35991035282823097</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.46079642929408698</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.66259161666688404</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.47810870452280202</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1.9610522800841199</v>
+      </c>
+      <c r="H4" s="4">
+        <v>2.1559429562824</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2.0096177497046601</v>
+      </c>
+      <c r="J4" s="4">
+        <v>2.0097379846867498</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2.0524180039959901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1.4747570562194501</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.73398195825967305</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.08709883720265</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.1836389635243401</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.78247034395426995</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2.82006288751891</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.6100697767788501</v>
+      </c>
+      <c r="I5" s="4">
+        <v>2.09739028674817</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2.6337594070980201</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1.36514490061639</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1.0161710383241001</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.0342646873054</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.71793632698781096</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.0542947593432199</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.0023135762464099</v>
+      </c>
+      <c r="G6" s="4">
+        <v>3.0928817134730799</v>
+      </c>
+      <c r="H6" s="4">
+        <v>3.5696054093707801</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2.8198163780585999</v>
+      </c>
+      <c r="J6" s="4">
+        <v>2.2590931033000099</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2.38501152371256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1.1151223337857401</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.2792805143267501</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.87897481111577</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.98136915761545196</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.33815352864208</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1.9470607042468999</v>
+      </c>
+      <c r="H7" s="4">
+        <v>2.4736805811335998</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1.6703402259037099</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1.9322172068694401</v>
+      </c>
+      <c r="K7" s="4">
+        <v>2.4314765970629701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1.74761216466142</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1.4868586538169499</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.2614791129446199</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.3036170440330199</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1.2132815168275499</v>
+      </c>
+      <c r="G8" s="4">
+        <v>3.8542593421858702</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2.89092042162968</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2.9502180762336301</v>
+      </c>
+      <c r="J8" s="4">
+        <v>2.7109416446082499</v>
+      </c>
+      <c r="K8" s="4">
+        <v>3.0725042316795101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1.85189080675054</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1.7385352348493499</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.3750011091357599</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.26277757664107</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1.2415166536353599</v>
+      </c>
+      <c r="G9" s="4">
+        <v>4.1452605998493404</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2.7358141564691998</v>
+      </c>
+      <c r="I9" s="4">
+        <v>3.0979688933104299</v>
+      </c>
+      <c r="J9" s="4">
+        <v>3.0281033527319701</v>
+      </c>
+      <c r="K9" s="4">
+        <v>3.1238187705385601</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1.97679262670811</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1.48925396389135</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.7101684398624799</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2.4298568445775501</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1.5265657854644199</v>
+      </c>
+      <c r="G10" s="4">
+        <v>3.5555312684255802</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2.29922526099825</v>
+      </c>
+      <c r="I10" s="4">
+        <v>3.4004030957965399</v>
+      </c>
+      <c r="J10" s="4">
+        <v>2.7497145625986801</v>
+      </c>
+      <c r="K10" s="4">
+        <v>2.34492708789496</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1.98794164871899</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1.4452995405815201</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1.87870698850846</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2.1921588181002298</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.5897135909865201</v>
+      </c>
+      <c r="G11" s="4">
+        <v>3.8923288322851302</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2.5712216238752101</v>
+      </c>
+      <c r="I11" s="4">
+        <v>3.7175992265697499</v>
+      </c>
+      <c r="J11" s="4">
+        <v>2.31608123932152</v>
+      </c>
+      <c r="K11" s="4">
+        <v>2.5301891591645198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1.5578572270605699</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1.2492072656320301</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.4424080858470201</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2.3352939038003502</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1.6355107214297999</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4.1239216644161001</v>
+      </c>
+      <c r="H12" s="4">
+        <v>4.2460893593343298</v>
+      </c>
+      <c r="I12" s="4">
+        <v>4.5094762478633497</v>
+      </c>
+      <c r="J12" s="4">
+        <v>3.3769044107591601</v>
+      </c>
+      <c r="K12" s="4">
+        <v>5.06599447760453</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.85426390610704706</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.60821230006258398</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.68258467389569499</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.69716072116411798</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.76839825743789802</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1.8839188871175401</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2.0959568776484399</v>
+      </c>
+      <c r="I13" s="4">
+        <v>2.1249824511533202</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1.70775349761882</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2.3375649811395398</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1.1325199112294899</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.71470687456903303</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.85811350345787296</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.73774511628560702</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.71780664894009505</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1.79795405652894</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2.35393989702454</v>
+      </c>
+      <c r="I14" s="4">
+        <v>2.0218708624509101</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1.6029045161250299</v>
+      </c>
+      <c r="K14" s="4">
+        <v>2.2969472211245798</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.99565034917530704</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.78920144245722801</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.93632879202242403</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.74527796278583003</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.70858487045619001</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1.82050284843821</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2.5070576078933602</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2.1720234675527599</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1.7092515832966499</v>
+      </c>
+      <c r="K15" s="4">
+        <v>2.34775733216477</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1.65747382849372</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1.4720255655275301</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1.3148131149453901</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.5492037880639</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1.36461128427615</v>
+      </c>
+      <c r="G16" s="4">
+        <v>3.8247402703765299</v>
+      </c>
+      <c r="H16" s="4">
+        <v>3.6721295886615302</v>
+      </c>
+      <c r="I16" s="4">
+        <v>3.4994863684481499</v>
+      </c>
+      <c r="J16" s="4">
+        <v>2.7013354249416901</v>
+      </c>
+      <c r="K16" s="4">
+        <v>3.33676031252122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4">
+        <v>4.7378789429838903</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.3671117296144999</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1.29556446490995</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2.1663525614369101</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1.3603814105504699</v>
+      </c>
+      <c r="G17" s="4">
+        <v>6.7470458375818998</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2.4983612040166299</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2.4945401238555398</v>
+      </c>
+      <c r="J17" s="4">
+        <v>2.67747561756509</v>
+      </c>
+      <c r="K17" s="4">
+        <v>2.3193612441749298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>5.1929149922600804</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1.41563405264134</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1.44395324347997</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2.2555416289773098</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1.40392628477809</v>
+      </c>
+      <c r="G18" s="4">
+        <v>6.6290864937861</v>
+      </c>
+      <c r="H18" s="4">
+        <v>2.17061392646078</v>
+      </c>
+      <c r="I18" s="4">
+        <v>2.2982210262791098</v>
+      </c>
+      <c r="J18" s="4">
+        <v>2.6148505538459701</v>
+      </c>
+      <c r="K18" s="4">
+        <v>2.2470406168733499</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>3.3260899139704998</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1.43625088119407</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1.19319036959152</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1.36501042019083</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1.3669574589570701</v>
+      </c>
+      <c r="G19" s="4">
+        <v>3.9832476186124901</v>
+      </c>
+      <c r="H19" s="4">
+        <v>2.8650957736902498</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2.9264073230000198</v>
+      </c>
+      <c r="J19" s="4">
+        <v>3.0106700630624799</v>
+      </c>
+      <c r="K19" s="4">
+        <v>3.23196308378362</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>2.50371136993608</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1.30249770647513</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1.03049480360595</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1.2830583156173501</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1.20042789707025</v>
+      </c>
+      <c r="G20" s="4">
+        <v>3.3264832384933798</v>
+      </c>
+      <c r="H20" s="4">
+        <v>2.6809462305538601</v>
+      </c>
+      <c r="I20" s="4">
+        <v>2.8992201282721699</v>
+      </c>
+      <c r="J20" s="4">
+        <v>2.8689095465812899</v>
+      </c>
+      <c r="K20" s="4">
+        <v>2.9862818124964199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1.5889374583235101</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.98007139467300097</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.91333319560551895</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1.02867179225378</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1.00662568992325</v>
+      </c>
+      <c r="G21" s="4">
+        <v>2.75704110784954</v>
+      </c>
+      <c r="H21" s="4">
+        <v>2.6710445350954601</v>
+      </c>
+      <c r="I21" s="4">
+        <v>2.3918748562115</v>
+      </c>
+      <c r="J21" s="4">
+        <v>2.4696116099780201</v>
+      </c>
+      <c r="K21" s="4">
+        <v>2.3957505606164702</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1.58711085467373</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.88561279606651999</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1.06754239345772</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1.79994255547351</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.99813399732442198</v>
+      </c>
+      <c r="G22" s="4">
+        <v>3.6842646762848199</v>
+      </c>
+      <c r="H22" s="4">
+        <v>3.2891534279840702</v>
+      </c>
+      <c r="I22" s="4">
+        <v>2.6846258398845002</v>
+      </c>
+      <c r="J22" s="4">
+        <v>4.1572253680875599</v>
+      </c>
+      <c r="K22" s="4">
+        <v>3.1411530873683802</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2.4110714463008001</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1.09668274504569</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1.6658687859354999</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1.15933600773324</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1.2844818968345499</v>
+      </c>
+      <c r="G23" s="4">
+        <v>3.4376094969164601</v>
+      </c>
+      <c r="H23" s="4">
+        <v>2.3455670050798201</v>
+      </c>
+      <c r="I23" s="4">
+        <v>2.6268572504845702</v>
+      </c>
+      <c r="J23" s="4">
+        <v>2.31001487738077</v>
+      </c>
+      <c r="K23" s="4">
+        <v>2.3069440306106701</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4">
+        <v>2.55493019540619</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1.3251289824490999</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1.6595151268467401</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1.92921556215302</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1.5326468387968699</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3.9347410623159398</v>
+      </c>
+      <c r="H24" s="4">
+        <v>2.8980178902865501</v>
+      </c>
+      <c r="I24" s="4">
+        <v>2.80656243323401</v>
+      </c>
+      <c r="J24" s="4">
+        <v>3.6155676157663099</v>
+      </c>
+      <c r="K24" s="4">
+        <v>2.8838213338172598</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1.98612794514394</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1.50846056486779</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1.40195111904643</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1.87267115377452</v>
+      </c>
+      <c r="F25" s="4">
+        <v>1.50962610276969</v>
+      </c>
+      <c r="G25" s="4">
+        <v>5.0707915685701499</v>
+      </c>
+      <c r="H25" s="4">
+        <v>5.94654380430097</v>
+      </c>
+      <c r="I25" s="4">
+        <v>5.6232532537062898</v>
+      </c>
+      <c r="J25" s="4">
+        <v>4.2589561316789402</v>
+      </c>
+      <c r="K25" s="4">
+        <v>3.7456913517371002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1.92764778180383</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1.54527329224483</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1.5589547572923299</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2.01971790796004</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1.8379586409264499</v>
+      </c>
+      <c r="G26" s="4">
+        <v>5.2078639892482004</v>
+      </c>
+      <c r="H26" s="4">
+        <v>5.9083466572263301</v>
+      </c>
+      <c r="I26" s="4">
+        <v>5.7914442713119803</v>
+      </c>
+      <c r="J26" s="4">
+        <v>4.4858001105542398</v>
+      </c>
+      <c r="K26" s="4">
+        <v>4.4320911625225996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="4">
+        <v>2.75782418619682</v>
+      </c>
+      <c r="C27" s="4">
+        <v>2.1476241686384898</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2.36224017507352</v>
+      </c>
+      <c r="E27" s="4">
+        <v>3.1487036140383302</v>
+      </c>
+      <c r="F27" s="4">
+        <v>2.5973904189703299</v>
+      </c>
+      <c r="G27" s="4">
+        <v>5.12454057017335</v>
+      </c>
+      <c r="H27" s="4">
+        <v>4.8552483606402399</v>
+      </c>
+      <c r="I27" s="4">
+        <v>4.7431986916207798</v>
+      </c>
+      <c r="J27" s="4">
+        <v>3.7832962481091199</v>
+      </c>
+      <c r="K27" s="4">
+        <v>3.4764213487531102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="4">
+        <v>3.2330942830758702</v>
+      </c>
+      <c r="C28" s="4">
+        <v>2.5577583184713002</v>
+      </c>
+      <c r="D28" s="4">
+        <v>2.3221224065888002</v>
+      </c>
+      <c r="E28" s="4">
+        <v>2.9320020521581398</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2.7729763141705099</v>
+      </c>
+      <c r="G28" s="4">
+        <v>5.9137763747831</v>
+      </c>
+      <c r="H28" s="4">
+        <v>5.5505927500307699</v>
+      </c>
+      <c r="I28" s="4">
+        <v>5.3080915455741398</v>
+      </c>
+      <c r="J28" s="4">
+        <v>3.4665543845086302</v>
+      </c>
+      <c r="K28" s="4">
+        <v>3.70336527042085</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1.8269775437509601</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1.5242431233145</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1.4575632609443601</v>
+      </c>
+      <c r="E29" s="4">
+        <v>2.2260572057348198</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2.2513201931800602</v>
+      </c>
+      <c r="G29" s="4">
+        <v>3.47065843251091</v>
+      </c>
+      <c r="H29" s="4">
+        <v>3.1388346857961098</v>
+      </c>
+      <c r="I29" s="4">
+        <v>3.7947675496617501</v>
+      </c>
+      <c r="J29" s="4">
+        <v>4.0848047842796502</v>
+      </c>
+      <c r="K29" s="4">
+        <v>2.9635618119455298</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1.7019734649687199</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1.84325111875839</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1.6053047731397501</v>
+      </c>
+      <c r="E30" s="4">
+        <v>2.2699674336210198</v>
+      </c>
+      <c r="F30" s="4">
+        <v>2.16769040227928</v>
+      </c>
+      <c r="G30" s="4">
+        <v>4.1011521019278199</v>
+      </c>
+      <c r="H30" s="4">
+        <v>4.6452501715453298</v>
+      </c>
+      <c r="I30" s="4">
+        <v>4.3175487534825097</v>
+      </c>
+      <c r="J30" s="4">
+        <v>4.2876615097480597</v>
+      </c>
+      <c r="K30" s="4">
+        <v>3.67366227201342</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="4">
+        <v>2.47715101403961</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1.4036480176103301</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1.2531559601286599</v>
+      </c>
+      <c r="E31" s="4">
+        <v>1.62029415922911</v>
+      </c>
+      <c r="F31" s="4">
+        <v>1.58897433497956</v>
+      </c>
+      <c r="G31" s="4">
+        <v>6.7964050299660901</v>
+      </c>
+      <c r="H31" s="4">
+        <v>6.0184144548066696</v>
+      </c>
+      <c r="I31" s="4">
+        <v>6.7119025356693696</v>
+      </c>
+      <c r="J31" s="4">
+        <v>6.7995700121117499</v>
+      </c>
+      <c r="K31" s="4">
+        <v>7.3563372774453901</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="4">
+        <v>3.1103729092469798</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1.3585084124135201</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1.5811085553291</v>
+      </c>
+      <c r="E32" s="4">
+        <v>1.8903080310601199</v>
+      </c>
+      <c r="F32" s="4">
+        <v>1.7216551917847001</v>
+      </c>
+      <c r="G32" s="4">
+        <v>7.17390718785225</v>
+      </c>
+      <c r="H32" s="4">
+        <v>6.7238484030253902</v>
+      </c>
+      <c r="I32" s="4">
+        <v>7.7698452579760398</v>
+      </c>
+      <c r="J32" s="4">
+        <v>7.2998401952804102</v>
+      </c>
+      <c r="K32" s="4">
+        <v>7.6807041964515603</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33" s="4">
+        <v>3.31824603156524</v>
+      </c>
+      <c r="C33" s="4">
+        <v>2.19317747843693</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1.3351289949388601</v>
+      </c>
+      <c r="E33" s="4">
+        <v>2.0434538834578202</v>
+      </c>
+      <c r="F33" s="4">
+        <v>1.35995436398306</v>
+      </c>
+      <c r="G33" s="4">
+        <v>4.8619588276150401</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1.80645111727275</v>
+      </c>
+      <c r="I33" s="4">
+        <v>2.1482469286030601</v>
+      </c>
+      <c r="J33" s="4">
+        <v>1.9492018651459</v>
+      </c>
+      <c r="K33" s="4">
+        <v>2.3333364901360198</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34" s="4">
+        <v>3.5277135575385001</v>
+      </c>
+      <c r="C34" s="4">
+        <v>1.8875392721697699</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1.2411881154190001</v>
+      </c>
+      <c r="E34" s="4">
+        <v>1.9408973065177499</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1.4046737588582601</v>
+      </c>
+      <c r="G34" s="4">
+        <v>4.5802109830582598</v>
+      </c>
+      <c r="H34" s="4">
+        <v>1.9996289746312399</v>
+      </c>
+      <c r="I34" s="4">
+        <v>1.97710376966057</v>
+      </c>
+      <c r="J34" s="4">
+        <v>2.2057816725811801</v>
+      </c>
+      <c r="K34" s="4">
+        <v>2.1447673479696299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="5">
+        <f>AVERAGE(B3:B34)</f>
+        <v>2.1608569443912509</v>
+      </c>
+      <c r="C35" s="5">
+        <f t="shared" ref="C35:K35" si="0">AVERAGE(C3:C34)</f>
+        <v>1.3324529761171526</v>
+      </c>
+      <c r="D35" s="5">
+        <f t="shared" si="0"/>
+        <v>1.3310873636012002</v>
+      </c>
+      <c r="E35" s="5">
+        <f t="shared" si="0"/>
+        <v>1.6506871460661214</v>
+      </c>
+      <c r="F35" s="5">
+        <f t="shared" si="0"/>
+        <v>1.3834303535662942</v>
+      </c>
+      <c r="G35" s="5">
+        <f t="shared" si="0"/>
+        <v>3.9782850039969104</v>
+      </c>
+      <c r="H35" s="5">
+        <f t="shared" si="0"/>
+        <v>3.2499505164941982</v>
+      </c>
+      <c r="I35" s="5">
+        <f t="shared" si="0"/>
+        <v>3.3200562465203212</v>
+      </c>
+      <c r="J35" s="5">
+        <f t="shared" si="0"/>
+        <v>3.0716129025073546</v>
+      </c>
+      <c r="K35" s="5">
+        <f t="shared" si="0"/>
+        <v>3.0807881057894173</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>